<commit_message>
[UPDATE] excel done, change new version
</commit_message>
<xml_diff>
--- a/Registro_proyecto_estadias_y_Reporte_de_asesorias_Instrucciones2022.xlsx
+++ b/Registro_proyecto_estadias_y_Reporte_de_asesorias_Instrucciones2022.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CDS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CDS\Downloads\estadias\Estadias-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,12 +19,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Formato de Asesorías'!$A$1:$M$42</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Registro proyecto de Estadias'!$A$1:$N$40</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mgVfqSkpxqery3yzutyu92QWd3U6w=="/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -60,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
   <si>
     <t>Registro del proyecto de estadías</t>
   </si>
@@ -74,19 +69,10 @@
     <t xml:space="preserve">Nombre del estudiante: </t>
   </si>
   <si>
-    <t>Iniciar con el nombre e incluir los dos apellidos</t>
-  </si>
-  <si>
     <t>Generación:</t>
   </si>
   <si>
-    <t>Generación institucional, ejemplo para TSU 32va., para ING 13va.</t>
-  </si>
-  <si>
     <t xml:space="preserve">      Matrícula:</t>
-  </si>
-  <si>
-    <t>Ejemplo: 20133MT024</t>
   </si>
   <si>
     <t xml:space="preserve">Nivel académico: </t>
@@ -95,43 +81,22 @@
     <t xml:space="preserve">Grado y Grupo: </t>
   </si>
   <si>
-    <t xml:space="preserve">Ejemplo: 6º. A, ING. 11º. A </t>
-  </si>
-  <si>
     <t xml:space="preserve">Carrera: </t>
-  </si>
-  <si>
-    <t>Nombre completo de la carrera sin abreviaturas (Ej. Negocios y Gestión Empresarial)</t>
   </si>
   <si>
     <t xml:space="preserve">     Área:</t>
   </si>
   <si>
-    <t>Ej. TSU: Automatización, ING. No aplica</t>
-  </si>
-  <si>
     <t>Empresa o Institución:</t>
-  </si>
-  <si>
-    <t>Razón de la empresa en donde se desarrolla la estadía</t>
   </si>
   <si>
     <t xml:space="preserve">Asesora / asesor empresarial: </t>
   </si>
   <si>
-    <t>Grado de estudios y nombre completo de la persona que asesora al alumno en la empresa</t>
-  </si>
-  <si>
     <t xml:space="preserve">Asesora /asesor universitario: </t>
   </si>
   <si>
-    <t>Grado de estudios y nombre completo de la persona que asesora al alumno en la UTEZ</t>
-  </si>
-  <si>
     <t>Fecha de Inicio:</t>
-  </si>
-  <si>
-    <t>dia/mes/año  (09/enero/2016)</t>
   </si>
   <si>
     <t>Fecha de término:</t>
@@ -146,22 +111,7 @@
     <t>Evidencias para medir resultados:</t>
   </si>
   <si>
-    <t>Debe ser concreto, no debe generar falsas espectativas, debe incliuir el verbo que indique la acción</t>
-  </si>
-  <si>
-    <t>a) Formato de asesorías.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Objetivo general: </t>
-  </si>
-  <si>
-    <t>b) Entrega de avaces del proyecto.</t>
-  </si>
-  <si>
-    <t>Debe iniciar con un verbo en infinitivo, indicar el alcance del proyecto y lo que se pretende obtener con su realización.</t>
-  </si>
-  <si>
-    <t>C) otros.</t>
   </si>
   <si>
     <t>.</t>
@@ -208,28 +158,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Debe iniciar con un verbo en infinitivo y referirse a las acciones </t>
-  </si>
-  <si>
     <t>programadas</t>
-  </si>
-  <si>
-    <t>para contribuir al logro del objetivo general</t>
-  </si>
-  <si>
-    <t>Fecha de termino de cada fase</t>
-  </si>
-  <si>
-    <t>1. Inicio.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dia/mes/año </t>
-  </si>
-  <si>
-    <t>2. Planeación.</t>
-  </si>
-  <si>
-    <t>Ejemplo: 20/enero/2016</t>
   </si>
   <si>
     <r>
@@ -251,22 +180,7 @@
     </r>
   </si>
   <si>
-    <t>3. Ejecución.</t>
-  </si>
-  <si>
-    <t>4. Control</t>
-  </si>
-  <si>
-    <t>Métodos y técnicas utilizados para alcanzar los objetivos.</t>
-  </si>
-  <si>
-    <t>5. Cierre</t>
-  </si>
-  <si>
     <t>Grado de estudios y nombre completo</t>
-  </si>
-  <si>
-    <t>Nombre completo y firma</t>
   </si>
   <si>
     <t>ASESORA / ASESOR EMPRESARIAL</t>
@@ -332,10 +246,94 @@
     <t>DIRECTOR / DIRECTORA DE CARRERA</t>
   </si>
   <si>
-    <t>Ejemplo para TSU: Técnico Superior Universitario, para ING: Ingeniería</t>
+    <t>Al:</t>
   </si>
   <si>
-    <t>Al:</t>
+    <t>Noe Martinez Flores</t>
+  </si>
+  <si>
+    <t>23va</t>
+  </si>
+  <si>
+    <t>Ingeniería en Desarrollo y Gestión de Software</t>
+  </si>
+  <si>
+    <t>Ingeniería</t>
+  </si>
+  <si>
+    <t>Universidad Tecnológica de Emiliano Zapata del Estado de Morelos</t>
+  </si>
+  <si>
+    <t>Sistema de Servicios Académicos de la Universidad de Ciencias Jurídicas de Morelos S.C. 
+Modulo Evaluación Docente</t>
+  </si>
+  <si>
+    <t>Implementar y gestionar eficientemente el proceso de evaluación docente en la Universidad de Ciencias Jurídicas mediante una aplicación híbrida, con el objetivo de facilitar a todos los docentes una retroalimentación directa por parte de los alumnos.</t>
+  </si>
+  <si>
+    <t>1.- Aplicación Hibrida</t>
+  </si>
+  <si>
+    <t>5.- Carta de liberación</t>
+  </si>
+  <si>
+    <t>I20203TN035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11º. A </t>
+  </si>
+  <si>
+    <t>Sin área</t>
+  </si>
+  <si>
+    <t>Definir la estructura óptima para almacenar información de las evaluación docente en la base de datos.</t>
+  </si>
+  <si>
+    <t>Crear API para gestionar y asegurar la integridad y disponibilidad de la información relacionada con la evaluación docente.</t>
+  </si>
+  <si>
+    <t>Crear una interfaz fácil de usar y accesible para estudiantes y evaluadores, facilitando la evaluación.</t>
+  </si>
+  <si>
+    <t>Ejecutar pruebas exhaustivas para garantizar la calidad y estabilidad de la aplicación</t>
+  </si>
+  <si>
+    <t>1.- Inicio
+2.- Requisitos
+3.- Análisis y Diseño
+4.- Desarrollo
+5.- Pruebas
+6.- Cierre</t>
+  </si>
+  <si>
+    <t>Implementar prototipos para el levantamiento de los requerimietos.</t>
+  </si>
+  <si>
+    <t>4.- Reporte de estadías</t>
+  </si>
+  <si>
+    <t>3.- Manual de usuario</t>
+  </si>
+  <si>
+    <t>2.- Reuniones de avance para el proyecto</t>
+  </si>
+  <si>
+    <t>DRA. MARTHA FABIOLA WENCES DÍAZ</t>
+  </si>
+  <si>
+    <t>I.T.I ERICK MIRELES MERCHANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizar levantamiento de requerimientos por medio de sesiones virtuales o entrevistas. </t>
+  </si>
+  <si>
+    <t>Dra. Martha Fabiola Wences Díaz</t>
+  </si>
+  <si>
+    <t>I.T.I Erick Mireles Merchant</t>
+  </si>
+  <si>
+    <t>Implementación del marco DMS</t>
   </si>
 </sst>
 </file>
@@ -345,7 +343,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-80A]d&quot; de &quot;mmmm&quot; de &quot;yyyy"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -391,11 +389,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -428,6 +421,51 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -437,7 +475,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -884,11 +922,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -904,31 +955,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -950,16 +976,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -969,7 +985,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -979,29 +995,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="11" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="10" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1015,50 +1010,234 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1071,127 +1250,69 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1201,23 +1322,44 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1732,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:N14"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1772,571 +1914,569 @@
     </row>
     <row r="2" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="85"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="132"/>
+      <c r="L2" s="133"/>
       <c r="M2" s="2"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="67"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="101"/>
       <c r="M3" s="4"/>
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="78"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
+      <c r="K4" s="136"/>
+      <c r="L4" s="137"/>
       <c r="M4" s="6"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="88" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="138" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="139"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="139"/>
+      <c r="J5" s="139"/>
+      <c r="K5" s="139"/>
+      <c r="L5" s="139"/>
+      <c r="M5" s="139"/>
+      <c r="N5" s="140"/>
+    </row>
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="90"/>
-    </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="125" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="143" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="91" t="s">
+      <c r="K6" s="143"/>
+      <c r="L6" s="143"/>
+      <c r="M6" s="141" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6" s="142"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="95" t="s">
+      <c r="C7" s="123"/>
+      <c r="D7" s="125" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="125"/>
+      <c r="F7" s="125"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="95"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="93" t="s">
+      <c r="L7" s="123"/>
+      <c r="M7" s="125" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" s="129"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="94"/>
-    </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="96" t="s">
+      <c r="C8" s="125" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="123"/>
+      <c r="H8" s="123"/>
+      <c r="I8" s="123"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="92"/>
-      <c r="D7" s="91" t="s">
+      <c r="L8" s="125" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8" s="123"/>
+      <c r="N8" s="124"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="45"/>
+      <c r="D9" s="122" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="123"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="123"/>
+      <c r="J9" s="123"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="123"/>
+      <c r="M9" s="123"/>
+      <c r="N9" s="124"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="125" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="123"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="123"/>
+      <c r="I10" s="123"/>
+      <c r="J10" s="123"/>
+      <c r="K10" s="123"/>
+      <c r="L10" s="123"/>
+      <c r="M10" s="123"/>
+      <c r="N10" s="124"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="122" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="123"/>
+      <c r="I11" s="123"/>
+      <c r="J11" s="123"/>
+      <c r="K11" s="123"/>
+      <c r="L11" s="123"/>
+      <c r="M11" s="123"/>
+      <c r="N11" s="124"/>
+    </row>
+    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="104" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="105"/>
+      <c r="D12" s="106">
+        <v>45300</v>
+      </c>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="48"/>
+      <c r="I12" s="107">
+        <v>45403</v>
+      </c>
+      <c r="J12" s="107"/>
+      <c r="K12" s="105"/>
+      <c r="L12" s="105"/>
+      <c r="M12" s="105"/>
+      <c r="N12" s="108"/>
+    </row>
+    <row r="13" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="14"/>
+    </row>
+    <row r="14" spans="1:14" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="109" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="110"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="111"/>
+      <c r="G14" s="112" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="113"/>
+      <c r="I14" s="113"/>
+      <c r="J14" s="113"/>
+      <c r="K14" s="113"/>
+      <c r="L14" s="113"/>
+      <c r="M14" s="113"/>
+      <c r="N14" s="113"/>
+    </row>
+    <row r="15" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="114" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="115"/>
+      <c r="I15" s="115"/>
+      <c r="J15" s="115"/>
+      <c r="K15" s="115"/>
+      <c r="L15" s="115"/>
+      <c r="M15" s="115"/>
+      <c r="N15" s="116"/>
+    </row>
+    <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="79" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="117"/>
+      <c r="G16" s="114" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="115"/>
+      <c r="I16" s="115"/>
+      <c r="J16" s="115"/>
+      <c r="K16" s="115"/>
+      <c r="L16" s="115"/>
+      <c r="M16" s="115"/>
+      <c r="N16" s="116"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="118"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="114" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="115"/>
+      <c r="I17" s="115"/>
+      <c r="J17" s="115"/>
+      <c r="K17" s="115"/>
+      <c r="L17" s="115"/>
+      <c r="M17" s="115"/>
+      <c r="N17" s="116"/>
+    </row>
+    <row r="18" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="114" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="126"/>
+      <c r="I18" s="126"/>
+      <c r="J18" s="126"/>
+      <c r="K18" s="126"/>
+      <c r="L18" s="126"/>
+      <c r="M18" s="126"/>
+      <c r="N18" s="127"/>
+    </row>
+    <row r="19" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="119"/>
+      <c r="C19" s="120"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="120"/>
+      <c r="F19" s="121"/>
+      <c r="G19" s="102" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="71"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="71"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="71"/>
+      <c r="N19" s="103"/>
+    </row>
+    <row r="20" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="66"/>
+      <c r="M20" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="61"/>
+    </row>
+    <row r="21" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="79" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="80"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="68"/>
+      <c r="K21" s="68"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" s="63"/>
+    </row>
+    <row r="22" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="79" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="86" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="88"/>
+      <c r="M22" s="95"/>
+      <c r="N22" s="96"/>
+    </row>
+    <row r="23" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="90"/>
+      <c r="L23" s="91"/>
+      <c r="M23" s="97"/>
+      <c r="N23" s="98"/>
+    </row>
+    <row r="24" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="79" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="84"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="84"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="89"/>
+      <c r="H24" s="90"/>
+      <c r="I24" s="90"/>
+      <c r="J24" s="90"/>
+      <c r="K24" s="90"/>
+      <c r="L24" s="91"/>
+      <c r="M24" s="97"/>
+      <c r="N24" s="98"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="90"/>
+      <c r="I25" s="90"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="90"/>
+      <c r="L25" s="91"/>
+      <c r="M25" s="97"/>
+      <c r="N25" s="98"/>
+    </row>
+    <row r="26" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="79" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="84"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="89"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="90"/>
+      <c r="L26" s="91"/>
+      <c r="M26" s="97"/>
+      <c r="N26" s="98"/>
+    </row>
+    <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="79" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="84"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="84"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="90"/>
+      <c r="L27" s="91"/>
+      <c r="M27" s="97"/>
+      <c r="N27" s="98"/>
+    </row>
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="92"/>
-      <c r="F7" s="92"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="98" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="92"/>
-      <c r="M7" s="91" t="s">
-        <v>11</v>
-      </c>
-      <c r="N7" s="97"/>
-    </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="91" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="92"/>
-      <c r="E8" s="92"/>
-      <c r="F8" s="92"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="91" t="s">
-        <v>15</v>
-      </c>
-      <c r="M8" s="92"/>
-      <c r="N8" s="99"/>
-    </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="100" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="92"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="92"/>
-      <c r="I9" s="92"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="92"/>
-      <c r="L9" s="92"/>
-      <c r="M9" s="92"/>
-      <c r="N9" s="99"/>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="91" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="92"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="92"/>
-      <c r="L10" s="92"/>
-      <c r="M10" s="92"/>
-      <c r="N10" s="99"/>
-    </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="92"/>
-      <c r="M11" s="92"/>
-      <c r="N11" s="99"/>
-    </row>
-    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="106" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="107"/>
-      <c r="D12" s="108" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
-      <c r="G12" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="109" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="109"/>
-      <c r="K12" s="107"/>
-      <c r="L12" s="107"/>
-      <c r="M12" s="107"/>
-      <c r="N12" s="110"/>
-    </row>
-    <row r="13" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="23"/>
-    </row>
-    <row r="14" spans="1:14" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="111" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="104"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="112" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="66"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="66"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="66"/>
-      <c r="N14" s="67"/>
-    </row>
-    <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="101" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="66"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="66"/>
-      <c r="L15" s="66"/>
-      <c r="M15" s="66"/>
-      <c r="N15" s="67"/>
-    </row>
-    <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="72" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="101" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="66"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="67"/>
-    </row>
-    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="113"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="102"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="66"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="67"/>
-    </row>
-    <row r="18" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="113"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="66"/>
-      <c r="L18" s="66"/>
-      <c r="M18" s="66"/>
-      <c r="N18" s="67"/>
-    </row>
-    <row r="19" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="114"/>
-      <c r="C19" s="104"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="104"/>
-      <c r="F19" s="105"/>
-      <c r="G19" s="103" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="104"/>
-      <c r="I19" s="104"/>
-      <c r="J19" s="104"/>
-      <c r="K19" s="104"/>
-      <c r="L19" s="104"/>
-      <c r="M19" s="104"/>
-      <c r="N19" s="105"/>
-    </row>
-    <row r="20" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="N20" s="29"/>
-    </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="N21" s="32"/>
-    </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="72" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="66"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="115"/>
-      <c r="H22" s="116"/>
-      <c r="I22" s="116"/>
-      <c r="J22" s="116"/>
-      <c r="K22" s="116"/>
-      <c r="L22" s="117"/>
-      <c r="M22" s="118" t="s">
-        <v>41</v>
-      </c>
-      <c r="N22" s="67"/>
-    </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="68" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="66"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="70" t="s">
-        <v>43</v>
-      </c>
-      <c r="N23" s="67"/>
-    </row>
-    <row r="24" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="66"/>
-      <c r="L24" s="69"/>
-      <c r="M24" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="N24" s="67"/>
-    </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="H25" s="66"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="66"/>
-      <c r="K25" s="66"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="71"/>
-      <c r="N25" s="67"/>
-    </row>
-    <row r="26" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="68" t="s">
-        <v>48</v>
-      </c>
-      <c r="H26" s="66"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="66"/>
-      <c r="K26" s="66"/>
-      <c r="L26" s="69"/>
-      <c r="M26" s="71"/>
-      <c r="N26" s="67"/>
-    </row>
-    <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="72" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27" s="66"/>
-      <c r="I27" s="66"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="66"/>
-      <c r="L27" s="69"/>
-      <c r="M27" s="71"/>
-      <c r="N27" s="67"/>
-    </row>
-    <row r="28" spans="1:14" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="65"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="66"/>
-      <c r="J28" s="66"/>
-      <c r="K28" s="66"/>
-      <c r="L28" s="69"/>
-      <c r="M28" s="71"/>
-      <c r="N28" s="67"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="90"/>
+      <c r="I28" s="90"/>
+      <c r="J28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="91"/>
+      <c r="M28" s="97"/>
+      <c r="N28" s="98"/>
     </row>
     <row r="29" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
-      <c r="B29" s="65"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="66"/>
-      <c r="J29" s="66"/>
-      <c r="K29" s="66"/>
-      <c r="L29" s="69"/>
-      <c r="M29" s="71"/>
-      <c r="N29" s="67"/>
-    </row>
-    <row r="30" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="144"/>
+      <c r="C29" s="177"/>
+      <c r="D29" s="177"/>
+      <c r="E29" s="177"/>
+      <c r="F29" s="178"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="90"/>
+      <c r="I29" s="90"/>
+      <c r="J29" s="90"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="91"/>
+      <c r="M29" s="97"/>
+      <c r="N29" s="98"/>
+    </row>
+    <row r="30" spans="1:14" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
-      <c r="B30" s="76"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="77"/>
-      <c r="J30" s="77"/>
-      <c r="K30" s="77"/>
-      <c r="L30" s="80"/>
-      <c r="M30" s="81"/>
-      <c r="N30" s="78"/>
+      <c r="B30" s="147"/>
+      <c r="C30" s="175"/>
+      <c r="D30" s="175"/>
+      <c r="E30" s="175"/>
+      <c r="F30" s="176"/>
+      <c r="G30" s="92"/>
+      <c r="H30" s="93"/>
+      <c r="I30" s="93"/>
+      <c r="J30" s="93"/>
+      <c r="K30" s="93"/>
+      <c r="L30" s="94"/>
+      <c r="M30" s="99"/>
+      <c r="N30" s="100"/>
     </row>
     <row r="31" spans="1:14" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
@@ -2356,78 +2496,78 @@
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
-      <c r="B32" s="82"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="66"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="66"/>
-      <c r="I32" s="66"/>
-      <c r="J32" s="66"/>
-      <c r="K32" s="66"/>
-      <c r="L32" s="75"/>
-      <c r="M32" s="66"/>
-      <c r="N32" s="66"/>
+      <c r="B32" s="148"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="145"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="75"/>
+      <c r="L32" s="146"/>
+      <c r="M32" s="75"/>
+      <c r="N32" s="75"/>
     </row>
     <row r="33" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="119" t="s">
-        <v>51</v>
+      <c r="B33" s="174" t="s">
+        <v>72</v>
       </c>
-      <c r="C33" s="104"/>
-      <c r="D33" s="104"/>
-      <c r="E33" s="104"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="120" t="s">
-        <v>52</v>
+      <c r="C33" s="120"/>
+      <c r="D33" s="120"/>
+      <c r="E33" s="120"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="72" t="s">
+        <v>48</v>
       </c>
-      <c r="H33" s="66"/>
-      <c r="I33" s="66"/>
-      <c r="J33" s="66"/>
-      <c r="K33" s="66"/>
-      <c r="L33" s="119" t="s">
-        <v>51</v>
+      <c r="H33" s="73"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="73"/>
+      <c r="L33" s="174" t="s">
+        <v>73</v>
       </c>
-      <c r="M33" s="104"/>
-      <c r="N33" s="104"/>
+      <c r="M33" s="120"/>
+      <c r="N33" s="120"/>
     </row>
     <row r="34" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
-      <c r="B34" s="121" t="s">
-        <v>53</v>
+      <c r="B34" s="74" t="s">
+        <v>26</v>
       </c>
-      <c r="C34" s="66"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="66"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="123" t="s">
-        <v>54</v>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="78" t="s">
+        <v>27</v>
       </c>
-      <c r="H34" s="123"/>
-      <c r="I34" s="123"/>
-      <c r="J34" s="123"/>
-      <c r="K34" s="63"/>
-      <c r="L34" s="122" t="s">
-        <v>55</v>
+      <c r="H34" s="78"/>
+      <c r="I34" s="78"/>
+      <c r="J34" s="78"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="76" t="s">
+        <v>28</v>
       </c>
-      <c r="M34" s="116"/>
-      <c r="N34" s="116"/>
+      <c r="M34" s="77"/>
+      <c r="N34" s="77"/>
     </row>
     <row r="35" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="38"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="38"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="23"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-      <c r="M35" s="38"/>
+      <c r="M35" s="23"/>
       <c r="N35" s="1"/>
     </row>
     <row r="36" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2479,20 +2619,25 @@
       <c r="N38" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="63">
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="G22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="G23:L23"/>
-    <mergeCell ref="M23:N23"/>
+  <mergeCells count="50">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="D5:N5"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="D9:N9"/>
+    <mergeCell ref="E10:N10"/>
+    <mergeCell ref="E11:N11"/>
+    <mergeCell ref="G16:N16"/>
+    <mergeCell ref="G17:N17"/>
     <mergeCell ref="G18:N18"/>
     <mergeCell ref="G19:N19"/>
     <mergeCell ref="B12:C12"/>
@@ -2502,47 +2647,29 @@
     <mergeCell ref="G14:N14"/>
     <mergeCell ref="G15:N15"/>
     <mergeCell ref="B16:F19"/>
-    <mergeCell ref="D9:N9"/>
-    <mergeCell ref="E10:N10"/>
-    <mergeCell ref="E11:N11"/>
-    <mergeCell ref="G16:N16"/>
-    <mergeCell ref="G17:N17"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="D5:N5"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="G22:L30"/>
+    <mergeCell ref="M22:N30"/>
     <mergeCell ref="B28:F28"/>
-    <mergeCell ref="G28:L28"/>
-    <mergeCell ref="M28:N28"/>
     <mergeCell ref="G32:K32"/>
     <mergeCell ref="L32:N32"/>
     <mergeCell ref="B29:F29"/>
-    <mergeCell ref="G29:L29"/>
-    <mergeCell ref="M29:N29"/>
     <mergeCell ref="B30:F30"/>
-    <mergeCell ref="G30:L30"/>
-    <mergeCell ref="M30:N30"/>
     <mergeCell ref="B32:E32"/>
-    <mergeCell ref="G26:L26"/>
-    <mergeCell ref="M26:N26"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B27:F27"/>
-    <mergeCell ref="G27:L27"/>
-    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="G20:L21"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="L33:N33"/>
     <mergeCell ref="B24:F24"/>
-    <mergeCell ref="G24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="G25:L25"/>
-    <mergeCell ref="M25:N25"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -2555,8 +2682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2608,18 +2735,18 @@
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="124" t="s">
-        <v>56</v>
+      <c r="B2" s="170" t="s">
+        <v>29</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="85"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="133"/>
       <c r="L2" s="2"/>
       <c r="M2" s="3"/>
       <c r="N2" s="1"/>
@@ -2638,18 +2765,18 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="86" t="s">
-        <v>57</v>
+      <c r="B3" s="134" t="s">
+        <v>30</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="67"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="101"/>
       <c r="L3" s="4"/>
       <c r="M3" s="5"/>
       <c r="N3" s="1"/>
@@ -2668,18 +2795,18 @@
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="135" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="78"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="136"/>
+      <c r="K4" s="137"/>
       <c r="L4" s="6"/>
       <c r="M4" s="7"/>
       <c r="N4" s="1"/>
@@ -2698,24 +2825,24 @@
     </row>
     <row r="5" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
-      <c r="B5" s="40" t="str">
+      <c r="B5" s="49" t="str">
         <f>'Registro proyecto de Estadias'!B5</f>
         <v xml:space="preserve">Nombre del estudiante: </v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="125" t="str">
+      <c r="C5" s="50"/>
+      <c r="D5" s="171" t="str">
         <f>'Registro proyecto de Estadias'!D5:N5</f>
-        <v>Iniciar con el nombre e incluir los dos apellidos</v>
+        <v>Noe Martinez Flores</v>
       </c>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="104"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="105"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="120"/>
+      <c r="H5" s="120"/>
+      <c r="I5" s="120"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="121"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
@@ -2732,29 +2859,29 @@
     </row>
     <row r="6" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
-      <c r="B6" s="41" t="s">
-        <v>5</v>
+      <c r="B6" s="51" t="s">
+        <v>4</v>
       </c>
-      <c r="C6" s="126" t="str">
+      <c r="C6" s="153" t="str">
         <f>'Registro proyecto de Estadias'!C6:I6</f>
-        <v>Generación institucional, ejemplo para TSU 32va., para ING 13va.</v>
+        <v>23va</v>
       </c>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="127" t="str">
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="172" t="str">
         <f>'Registro proyecto de Estadias'!J6</f>
         <v xml:space="preserve">      Matrícula:</v>
       </c>
-      <c r="K6" s="92"/>
-      <c r="L6" s="128" t="str">
+      <c r="K6" s="123"/>
+      <c r="L6" s="173" t="str">
         <f>'Registro proyecto de Estadias'!M6</f>
-        <v>Ejemplo: 20133MT024</v>
+        <v>I20203TN035</v>
       </c>
-      <c r="M6" s="99"/>
+      <c r="M6" s="124"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
@@ -2771,30 +2898,30 @@
     </row>
     <row r="7" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="43" t="str">
+      <c r="B7" s="52" t="str">
         <f>'Registro proyecto de Estadias'!B7:C7</f>
         <v xml:space="preserve">Nivel académico: </v>
       </c>
-      <c r="C7" s="126" t="str">
+      <c r="C7" s="153" t="str">
         <f>'Registro proyecto de Estadias'!D7</f>
-        <v>Ejemplo para TSU: Técnico Superior Universitario, para ING: Ingeniería</v>
+        <v>Ingeniería</v>
       </c>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="64" t="str">
+      <c r="D7" s="153"/>
+      <c r="E7" s="153"/>
+      <c r="F7" s="153"/>
+      <c r="G7" s="153"/>
+      <c r="H7" s="153"/>
+      <c r="I7" s="153"/>
+      <c r="J7" s="153"/>
+      <c r="K7" s="53" t="str">
         <f>'Registro proyecto de Estadias'!K7:L7</f>
         <v xml:space="preserve">Grado y Grupo: </v>
       </c>
-      <c r="L7" s="126" t="str">
+      <c r="L7" s="153" t="str">
         <f>'Registro proyecto de Estadias'!M7</f>
-        <v xml:space="preserve">Ejemplo: 6º. A, ING. 11º. A </v>
+        <v xml:space="preserve">11º. A </v>
       </c>
-      <c r="M7" s="130"/>
+      <c r="M7" s="169"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
@@ -2811,30 +2938,30 @@
     </row>
     <row r="8" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
-      <c r="B8" s="41" t="str">
+      <c r="B8" s="51" t="str">
         <f>'Registro proyecto de Estadias'!B8</f>
         <v xml:space="preserve">Carrera: </v>
       </c>
-      <c r="C8" s="126" t="str">
+      <c r="C8" s="153" t="str">
         <f>'Registro proyecto de Estadias'!C8</f>
-        <v>Nombre completo de la carrera sin abreviaturas (Ej. Negocios y Gestión Empresarial)</v>
+        <v>Ingeniería en Desarrollo y Gestión de Software</v>
       </c>
-      <c r="D8" s="92"/>
-      <c r="E8" s="92"/>
-      <c r="F8" s="92"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="42" t="str">
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="123"/>
+      <c r="H8" s="123"/>
+      <c r="I8" s="123"/>
+      <c r="J8" s="123"/>
+      <c r="K8" s="54" t="str">
         <f>'Registro proyecto de Estadias'!K8</f>
         <v xml:space="preserve">     Área:</v>
       </c>
-      <c r="L8" s="126" t="str">
+      <c r="L8" s="153" t="str">
         <f>'Registro proyecto de Estadias'!L8</f>
-        <v>Ej. TSU: Automatización, ING. No aplica</v>
+        <v>Sin área</v>
       </c>
-      <c r="M8" s="99"/>
+      <c r="M8" s="124"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
@@ -2851,24 +2978,24 @@
     </row>
     <row r="9" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="41" t="str">
+      <c r="B9" s="51" t="str">
         <f>'Registro proyecto de Estadias'!B9</f>
         <v>Empresa o Institución:</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="129" t="str">
+      <c r="C9" s="55"/>
+      <c r="D9" s="154" t="str">
         <f>'Registro proyecto de Estadias'!D9:N9</f>
-        <v>Razón de la empresa en donde se desarrolla la estadía</v>
+        <v>Universidad Tecnológica de Emiliano Zapata del Estado de Morelos</v>
       </c>
-      <c r="E9" s="92"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="92"/>
-      <c r="I9" s="92"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="92"/>
-      <c r="L9" s="92"/>
-      <c r="M9" s="99"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="123"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="123"/>
+      <c r="J9" s="123"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="123"/>
+      <c r="M9" s="124"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
@@ -2885,24 +3012,24 @@
     </row>
     <row r="10" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="B10" s="41" t="str">
+      <c r="B10" s="51" t="str">
         <f>'Registro proyecto de Estadias'!B10</f>
         <v xml:space="preserve">Asesora / asesor empresarial: </v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="126" t="str">
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="153" t="str">
         <f>'Registro proyecto de Estadias'!E10</f>
-        <v>Grado de estudios y nombre completo de la persona que asesora al alumno en la empresa</v>
+        <v>DRA. MARTHA FABIOLA WENCES DÍAZ</v>
       </c>
-      <c r="F10" s="92"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="92"/>
-      <c r="L10" s="92"/>
-      <c r="M10" s="99"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="123"/>
+      <c r="I10" s="123"/>
+      <c r="J10" s="123"/>
+      <c r="K10" s="123"/>
+      <c r="L10" s="123"/>
+      <c r="M10" s="124"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
@@ -2919,24 +3046,24 @@
     </row>
     <row r="11" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
-      <c r="B11" s="41" t="str">
+      <c r="B11" s="51" t="str">
         <f>'Registro proyecto de Estadias'!B11</f>
         <v xml:space="preserve">Asesora /asesor universitario: </v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="129" t="str">
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="154" t="str">
         <f>'Registro proyecto de Estadias'!E11:N11</f>
-        <v>Grado de estudios y nombre completo de la persona que asesora al alumno en la UTEZ</v>
+        <v>I.T.I ERICK MIRELES MERCHANT</v>
       </c>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="92"/>
-      <c r="M11" s="99"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="123"/>
+      <c r="I11" s="123"/>
+      <c r="J11" s="123"/>
+      <c r="K11" s="123"/>
+      <c r="L11" s="123"/>
+      <c r="M11" s="124"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
@@ -2953,23 +3080,24 @@
     </row>
     <row r="12" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
-      <c r="B12" s="135" t="s">
-        <v>26</v>
+      <c r="B12" s="160" t="s">
+        <v>16</v>
       </c>
-      <c r="C12" s="116"/>
-      <c r="D12" s="136" t="str">
+      <c r="C12" s="161"/>
+      <c r="D12" s="162" t="str">
         <f>'Registro proyecto de Estadias'!B14</f>
-        <v>Debe ser concreto, no debe generar falsas espectativas, debe incliuir el verbo que indique la acción</v>
+        <v>Sistema de Servicios Académicos de la Universidad de Ciencias Jurídicas de Morelos S.C. 
+Modulo Evaluación Docente</v>
       </c>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="116"/>
-      <c r="H12" s="116"/>
-      <c r="I12" s="116"/>
-      <c r="J12" s="116"/>
-      <c r="K12" s="116"/>
-      <c r="L12" s="116"/>
-      <c r="M12" s="137"/>
+      <c r="E12" s="161"/>
+      <c r="F12" s="161"/>
+      <c r="G12" s="161"/>
+      <c r="H12" s="161"/>
+      <c r="I12" s="161"/>
+      <c r="J12" s="161"/>
+      <c r="K12" s="161"/>
+      <c r="L12" s="161"/>
+      <c r="M12" s="163"/>
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
@@ -2986,18 +3114,18 @@
     </row>
     <row r="13" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
-      <c r="B13" s="114"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="104"/>
-      <c r="H13" s="104"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="104"/>
-      <c r="K13" s="104"/>
-      <c r="L13" s="104"/>
-      <c r="M13" s="105"/>
+      <c r="B13" s="119"/>
+      <c r="C13" s="120"/>
+      <c r="D13" s="120"/>
+      <c r="E13" s="120"/>
+      <c r="F13" s="120"/>
+      <c r="G13" s="120"/>
+      <c r="H13" s="120"/>
+      <c r="I13" s="120"/>
+      <c r="J13" s="120"/>
+      <c r="K13" s="120"/>
+      <c r="L13" s="120"/>
+      <c r="M13" s="121"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
@@ -3014,27 +3142,27 @@
     </row>
     <row r="14" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
-      <c r="B14" s="106" t="s">
-        <v>58</v>
+      <c r="B14" s="104" t="s">
+        <v>31</v>
       </c>
-      <c r="C14" s="107"/>
-      <c r="D14" s="138" t="str">
+      <c r="C14" s="105"/>
+      <c r="D14" s="164">
         <f>'Registro proyecto de Estadias'!D12:F12</f>
-        <v>dia/mes/año  (09/enero/2016)</v>
+        <v>45300</v>
       </c>
-      <c r="E14" s="107"/>
-      <c r="F14" s="107"/>
-      <c r="G14" s="16" t="s">
-        <v>75</v>
+      <c r="E14" s="105"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="47" t="s">
+        <v>47</v>
       </c>
-      <c r="H14" s="47"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="138" t="s">
-        <v>25</v>
+      <c r="H14" s="57"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="164" t="s">
+        <v>15</v>
       </c>
-      <c r="K14" s="107"/>
-      <c r="L14" s="107"/>
-      <c r="M14" s="49"/>
+      <c r="K14" s="105"/>
+      <c r="L14" s="105"/>
+      <c r="M14" s="59"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
@@ -3051,28 +3179,28 @@
     </row>
     <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
-      <c r="B15" s="139" t="s">
-        <v>59</v>
+      <c r="B15" s="165" t="s">
+        <v>32</v>
       </c>
-      <c r="C15" s="131" t="s">
-        <v>60</v>
+      <c r="C15" s="155" t="s">
+        <v>33</v>
       </c>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="85"/>
-      <c r="G15" s="141" t="s">
-        <v>61</v>
+      <c r="D15" s="132"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="133"/>
+      <c r="G15" s="167" t="s">
+        <v>34</v>
       </c>
-      <c r="H15" s="85"/>
-      <c r="I15" s="131" t="s">
-        <v>62</v>
+      <c r="H15" s="133"/>
+      <c r="I15" s="155" t="s">
+        <v>35</v>
       </c>
-      <c r="J15" s="84"/>
-      <c r="K15" s="85"/>
-      <c r="L15" s="141" t="s">
-        <v>63</v>
+      <c r="J15" s="132"/>
+      <c r="K15" s="133"/>
+      <c r="L15" s="167" t="s">
+        <v>36</v>
       </c>
-      <c r="M15" s="85"/>
+      <c r="M15" s="133"/>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
@@ -3089,18 +3217,18 @@
     </row>
     <row r="16" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
-      <c r="B16" s="140"/>
-      <c r="C16" s="132"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="132"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="132"/>
-      <c r="J16" s="77"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="132"/>
-      <c r="M16" s="78"/>
+      <c r="B16" s="166"/>
+      <c r="C16" s="156"/>
+      <c r="D16" s="136"/>
+      <c r="E16" s="136"/>
+      <c r="F16" s="137"/>
+      <c r="G16" s="156"/>
+      <c r="H16" s="137"/>
+      <c r="I16" s="156"/>
+      <c r="J16" s="136"/>
+      <c r="K16" s="137"/>
+      <c r="L16" s="156"/>
+      <c r="M16" s="137"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
@@ -3117,26 +3245,26 @@
     </row>
     <row r="17" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
-      <c r="B17" s="50">
+      <c r="B17" s="26">
         <v>42378</v>
       </c>
-      <c r="C17" s="133" t="s">
-        <v>64</v>
+      <c r="C17" s="157" t="s">
+        <v>37</v>
       </c>
-      <c r="D17" s="89"/>
-      <c r="E17" s="89"/>
-      <c r="F17" s="134"/>
-      <c r="G17" s="142" t="s">
-        <v>65</v>
+      <c r="D17" s="158"/>
+      <c r="E17" s="158"/>
+      <c r="F17" s="159"/>
+      <c r="G17" s="168" t="s">
+        <v>38</v>
       </c>
-      <c r="H17" s="134"/>
-      <c r="I17" s="142" t="s">
-        <v>66</v>
+      <c r="H17" s="159"/>
+      <c r="I17" s="168" t="s">
+        <v>39</v>
       </c>
-      <c r="J17" s="89"/>
-      <c r="K17" s="134"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="52"/>
+      <c r="J17" s="158"/>
+      <c r="K17" s="159"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="28"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
@@ -3153,18 +3281,18 @@
     </row>
     <row r="18" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="144"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="56"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="149"/>
+      <c r="H18" s="150"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="32"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -3181,18 +3309,18 @@
     </row>
     <row r="19" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="143"/>
-      <c r="H19" s="144"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="55"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="56"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="149"/>
+      <c r="H19" s="150"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="32"/>
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
@@ -3209,18 +3337,18 @@
     </row>
     <row r="20" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="144"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="56"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="149"/>
+      <c r="H20" s="150"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="32"/>
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
@@ -3237,18 +3365,18 @@
     </row>
     <row r="21" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="143"/>
-      <c r="H21" s="144"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="56"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="149"/>
+      <c r="H21" s="150"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="32"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
@@ -3265,18 +3393,18 @@
     </row>
     <row r="22" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="143"/>
-      <c r="H22" s="144"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="56"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="149"/>
+      <c r="H22" s="150"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="32"/>
       <c r="N22" s="8"/>
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
@@ -3293,18 +3421,18 @@
     </row>
     <row r="23" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="143"/>
-      <c r="H23" s="144"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="56"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="149"/>
+      <c r="H23" s="150"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="32"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
@@ -3321,18 +3449,18 @@
     </row>
     <row r="24" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="143"/>
-      <c r="H24" s="144"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="55"/>
-      <c r="L24" s="45"/>
-      <c r="M24" s="56"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="149"/>
+      <c r="H24" s="150"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="32"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
@@ -3349,18 +3477,18 @@
     </row>
     <row r="25" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="143"/>
-      <c r="H25" s="144"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="56"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="149"/>
+      <c r="H25" s="150"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="32"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
@@ -3377,18 +3505,18 @@
     </row>
     <row r="26" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="143"/>
-      <c r="H26" s="144"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="56"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="149"/>
+      <c r="H26" s="150"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="32"/>
       <c r="N26" s="8"/>
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
@@ -3405,18 +3533,18 @@
     </row>
     <row r="27" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="143"/>
-      <c r="H27" s="144"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="55"/>
-      <c r="L27" s="45"/>
-      <c r="M27" s="56"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="149"/>
+      <c r="H27" s="150"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="32"/>
       <c r="N27" s="8"/>
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
@@ -3433,18 +3561,18 @@
     </row>
     <row r="28" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="143"/>
-      <c r="H28" s="144"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="56"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="149"/>
+      <c r="H28" s="150"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="32"/>
       <c r="N28" s="8"/>
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
@@ -3461,18 +3589,18 @@
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="143"/>
-      <c r="H29" s="144"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="55"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="56"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="149"/>
+      <c r="H29" s="150"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="32"/>
       <c r="N29" s="8"/>
       <c r="O29" s="8"/>
       <c r="P29" s="8"/>
@@ -3489,18 +3617,18 @@
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="143"/>
-      <c r="H30" s="144"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="56"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="149"/>
+      <c r="H30" s="150"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="32"/>
       <c r="N30" s="8"/>
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
@@ -3517,18 +3645,18 @@
     </row>
     <row r="31" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="143"/>
-      <c r="H31" s="144"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="56"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="149"/>
+      <c r="H31" s="150"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="32"/>
       <c r="N31" s="8"/>
       <c r="O31" s="8"/>
       <c r="P31" s="8"/>
@@ -3545,18 +3673,18 @@
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
-      <c r="B32" s="53"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="143"/>
-      <c r="H32" s="144"/>
-      <c r="I32" s="54"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="45"/>
-      <c r="M32" s="56"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="149"/>
+      <c r="H32" s="150"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="32"/>
       <c r="N32" s="8"/>
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
@@ -3573,18 +3701,18 @@
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="143"/>
-      <c r="H33" s="144"/>
-      <c r="I33" s="54"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="45"/>
-      <c r="M33" s="56"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="149"/>
+      <c r="H33" s="150"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="32"/>
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
       <c r="P33" s="8"/>
@@ -3601,18 +3729,18 @@
     </row>
     <row r="34" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="8"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="146"/>
-      <c r="H34" s="147"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="59"/>
-      <c r="K34" s="60"/>
-      <c r="L34" s="59"/>
-      <c r="M34" s="61"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="151"/>
+      <c r="H34" s="152"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="37"/>
       <c r="N34" s="8"/>
       <c r="O34" s="8"/>
       <c r="P34" s="8"/>
@@ -3631,22 +3759,22 @@
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
-      <c r="D35" s="62" t="s">
-        <v>67</v>
+      <c r="D35" s="38" t="s">
+        <v>40</v>
       </c>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62" t="s">
-        <v>68</v>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38" t="s">
+        <v>41</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
-      <c r="I35" s="62" t="s">
-        <v>69</v>
+      <c r="I35" s="38" t="s">
+        <v>42</v>
       </c>
-      <c r="J35" s="62"/>
+      <c r="J35" s="38"/>
       <c r="K35" s="8"/>
-      <c r="L35" s="62" t="s">
-        <v>70</v>
+      <c r="L35" s="38" t="s">
+        <v>43</v>
       </c>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
@@ -3667,19 +3795,19 @@
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62" t="s">
-        <v>71</v>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38" t="s">
+        <v>44</v>
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="62" t="s">
-        <v>72</v>
+      <c r="I36" s="38" t="s">
+        <v>45</v>
       </c>
-      <c r="J36" s="62"/>
+      <c r="J36" s="38"/>
       <c r="K36" s="8"/>
-      <c r="L36" s="62"/>
+      <c r="L36" s="38"/>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
@@ -3698,20 +3826,20 @@
     <row r="37" spans="1:26" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
-      <c r="C37" s="119" t="s">
-        <v>51</v>
+      <c r="C37" s="70" t="s">
+        <v>25</v>
       </c>
-      <c r="D37" s="104"/>
-      <c r="E37" s="104"/>
-      <c r="F37" s="104"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
-      <c r="I37" s="119" t="s">
-        <v>51</v>
+      <c r="I37" s="70" t="s">
+        <v>25</v>
       </c>
-      <c r="J37" s="104"/>
-      <c r="K37" s="104"/>
-      <c r="L37" s="104"/>
+      <c r="J37" s="71"/>
+      <c r="K37" s="71"/>
+      <c r="L37" s="71"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
       <c r="O37" s="8"/>
@@ -3730,20 +3858,20 @@
     <row r="38" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
-      <c r="C38" s="145" t="s">
-        <v>55</v>
+      <c r="C38" s="65" t="s">
+        <v>28</v>
       </c>
-      <c r="D38" s="116"/>
-      <c r="E38" s="116"/>
-      <c r="F38" s="116"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="77"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
-      <c r="I38" s="145" t="s">
-        <v>73</v>
+      <c r="I38" s="65" t="s">
+        <v>46</v>
       </c>
-      <c r="J38" s="116"/>
-      <c r="K38" s="116"/>
-      <c r="L38" s="116"/>
+      <c r="J38" s="77"/>
+      <c r="K38" s="77"/>
+      <c r="L38" s="77"/>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
       <c r="O38" s="8"/>
@@ -30697,27 +30825,18 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="I37:L37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="I38:L38"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="D5:M5"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="C8:J8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="D9:M9"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="L7:M7"/>
     <mergeCell ref="E10:M10"/>
     <mergeCell ref="E11:M11"/>
     <mergeCell ref="C15:F16"/>
@@ -30733,18 +30852,27 @@
     <mergeCell ref="I15:K16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="I17:K17"/>
-    <mergeCell ref="C8:J8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="D9:M9"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="D5:M5"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="I37:L37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="I38:L38"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>

</xml_diff>